<commit_message>
detach mark debug, add index to Data frame sheet
</commit_message>
<xml_diff>
--- a/project_tcl/ZCU111/MinimumTrigger/MinimumTrigger_DataFrame.xlsx
+++ b/project_tcl/ZCU111/MinimumTrigger/MinimumTrigger_DataFrame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoGURA\KRD\project_tcl\ZCU111\MinimumTrigger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B7DC66-2D70-4BBF-BEA9-C7945E82B724}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CC943AB-D964-4DC4-987C-B6BCE0E6A796}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{47A0C5A6-AF27-41FE-9D29-76E50A9C23F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="49">
   <si>
     <t>HEADER</t>
     <phoneticPr fontId="1"/>
@@ -156,6 +156,70 @@
   </si>
   <si>
     <t>Frame Length[11:0]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[0:3]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[4:7]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[8:11]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[12:15]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[16:19]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[20:23]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[24:27]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[28:31]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[32:35]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[36:39]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[40:43]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[44:47]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[48:51]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[52:55]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[56:59]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[60:63]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -490,11 +554,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -502,26 +599,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -529,56 +632,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,7 +961,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="C11" sqref="C11:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -911,8 +975,7 @@
     <col min="12" max="14" width="7.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.5" customWidth="1"/>
-    <col min="18" max="18" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="7.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.4">
@@ -920,8 +983,58 @@
         <v>31</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="C2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="3" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -983,155 +1096,155 @@
       <c r="B4">
         <v>63</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="6" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5" t="s">
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="10">
+      <c r="Q4" s="16"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="20"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="23" t="s">
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="20" t="s">
+      <c r="L5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="20"/>
-      <c r="N5" s="22"/>
-      <c r="O5" s="23" t="s">
+      <c r="M5" s="29"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="24"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="31"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="17" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="17" t="s">
+      <c r="I6" s="26"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="13"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="17" t="s">
+      <c r="M6" s="26"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="13" t="s">
+      <c r="P6" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="18"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="28"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="8"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="14"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="26" t="s">
+      <c r="H8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="26"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="28" t="s">
+      <c r="I8" s="23"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="26" t="s">
+      <c r="L8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M8" s="26"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="28" t="s">
+      <c r="M8" s="23"/>
+      <c r="N8" s="24"/>
+      <c r="O8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="26" t="s">
+      <c r="P8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="26"/>
-      <c r="R8" s="29"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="25"/>
     </row>
     <row r="9" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
@@ -1140,38 +1253,38 @@
       <c r="B9">
         <v>63</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="9" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30" t="s">
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30" t="s">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="31"/>
-      <c r="S9" s="10">
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1224,6 +1337,56 @@
       </c>
       <c r="S10" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
@@ -1233,6 +1396,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="P5:R5"/>
+    <mergeCell ref="H4:O4"/>
     <mergeCell ref="C7:R7"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="O9:R9"/>
@@ -1249,10 +1416,6 @@
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="P6:R6"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="P5:R5"/>
-    <mergeCell ref="H4:O4"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>